<commit_message>
update: Update plantilla inventario
</commit_message>
<xml_diff>
--- a/public/plantilla_inventario.xlsx
+++ b/public/plantilla_inventario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/albertosalles/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D9844C-0651-3C45-BB71-D4940257A84C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AE89E3-CE2F-4840-A9C9-8A0B77AF26AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-640" windowWidth="23600" windowHeight="16400" xr2:uid="{2EEC8CA2-C621-4D5E-B317-370CE4EF6140}"/>
+    <workbookView xWindow="4320" yWindow="600" windowWidth="24480" windowHeight="16180" activeTab="1" xr2:uid="{2EEC8CA2-C621-4D5E-B317-370CE4EF6140}"/>
   </bookViews>
   <sheets>
     <sheet name="PLANTILLA JUMPERS" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="78">
   <si>
     <t>INICIO PARTIDO</t>
   </si>
@@ -267,6 +267,9 @@
   </si>
   <si>
     <t>JAMON</t>
+  </si>
+  <si>
+    <t>CONOS</t>
   </si>
 </sst>
 </file>
@@ -550,7 +553,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -625,12 +628,6 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -951,7 +948,7 @@
   </sheetPr>
   <dimension ref="A1:V40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A18" sqref="A18:U20"/>
     </sheetView>
   </sheetViews>
@@ -1134,203 +1131,203 @@
       </c>
     </row>
     <row r="6" spans="1:22" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="38"/>
-      <c r="N6" s="38"/>
-      <c r="O6" s="38"/>
-      <c r="P6" s="38"/>
-      <c r="Q6" s="38"/>
-      <c r="R6" s="38"/>
-      <c r="S6" s="38"/>
-      <c r="T6" s="38"/>
-      <c r="U6" s="38"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
       <c r="V6" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:22" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
-      <c r="N7" s="38"/>
-      <c r="O7" s="38"/>
-      <c r="P7" s="38"/>
-      <c r="Q7" s="38"/>
-      <c r="R7" s="38"/>
-      <c r="S7" s="38"/>
-      <c r="T7" s="38"/>
-      <c r="U7" s="38"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
       <c r="V7" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:22" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="38"/>
-      <c r="N8" s="38"/>
-      <c r="O8" s="38"/>
-      <c r="P8" s="38"/>
-      <c r="Q8" s="38"/>
-      <c r="R8" s="38"/>
-      <c r="S8" s="38"/>
-      <c r="T8" s="38"/>
-      <c r="U8" s="38"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
       <c r="V8" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:22" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="38"/>
-      <c r="M9" s="38"/>
-      <c r="N9" s="38"/>
-      <c r="O9" s="38"/>
-      <c r="P9" s="38"/>
-      <c r="Q9" s="38"/>
-      <c r="R9" s="38"/>
-      <c r="S9" s="38"/>
-      <c r="T9" s="38"/>
-      <c r="U9" s="38"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
       <c r="V9" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:22" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="38"/>
-      <c r="O10" s="38"/>
-      <c r="P10" s="38"/>
-      <c r="Q10" s="38"/>
-      <c r="R10" s="38"/>
-      <c r="S10" s="38"/>
-      <c r="T10" s="38"/>
-      <c r="U10" s="38"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
       <c r="V10" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:22" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="38"/>
-      <c r="N11" s="38"/>
-      <c r="O11" s="38"/>
-      <c r="P11" s="38"/>
-      <c r="Q11" s="38"/>
-      <c r="R11" s="38"/>
-      <c r="S11" s="38"/>
-      <c r="T11" s="38"/>
-      <c r="U11" s="38"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
       <c r="V11" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:22" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="38"/>
-      <c r="N12" s="38"/>
-      <c r="O12" s="38"/>
-      <c r="P12" s="38"/>
-      <c r="Q12" s="38"/>
-      <c r="R12" s="38"/>
-      <c r="S12" s="38"/>
-      <c r="T12" s="38"/>
-      <c r="U12" s="38"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
       <c r="V12" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1469,87 +1466,87 @@
       </c>
     </row>
     <row r="18" spans="1:22" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="38"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="38"/>
-      <c r="L18" s="38"/>
-      <c r="M18" s="38"/>
-      <c r="N18" s="38"/>
-      <c r="O18" s="38"/>
-      <c r="P18" s="38"/>
-      <c r="Q18" s="38"/>
-      <c r="R18" s="38"/>
-      <c r="S18" s="38"/>
-      <c r="T18" s="38"/>
-      <c r="U18" s="38"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="7"/>
       <c r="V18" s="7">
         <f t="shared" ref="V18:V22" si="1">SUM(B18:U18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:22" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="38"/>
-      <c r="K19" s="38"/>
-      <c r="L19" s="38"/>
-      <c r="M19" s="38"/>
-      <c r="N19" s="38"/>
-      <c r="O19" s="38"/>
-      <c r="P19" s="38"/>
-      <c r="Q19" s="38"/>
-      <c r="R19" s="38"/>
-      <c r="S19" s="38"/>
-      <c r="T19" s="38"/>
-      <c r="U19" s="38"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
       <c r="V19" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:22" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="38"/>
-      <c r="M20" s="38"/>
-      <c r="N20" s="38"/>
-      <c r="O20" s="38"/>
-      <c r="P20" s="38"/>
-      <c r="Q20" s="38"/>
-      <c r="R20" s="38"/>
-      <c r="S20" s="38"/>
-      <c r="T20" s="38"/>
-      <c r="U20" s="38"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7"/>
       <c r="V20" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2282,8 +2279,8 @@
   </sheetPr>
   <dimension ref="A1:W37"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2466,7 +2463,7 @@
     </row>
     <row r="6" spans="1:22" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>

</xml_diff>